<commit_message>
forgot password page update
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 ForgotPasswordPage, Jonnie Leathem.xlsx
+++ b/Testing Spreadsheet v1.0 ForgotPasswordPage, Jonnie Leathem.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="97">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -439,15 +439,6 @@
     <t>TCase_6</t>
   </si>
   <si>
-    <t>ForgotPassword_Tproc_1</t>
-  </si>
-  <si>
-    <t>ForgotPassword_Tproc_2</t>
-  </si>
-  <si>
-    <t>ForgotPassword_Tproc_3</t>
-  </si>
-  <si>
     <t>4.1.24</t>
   </si>
   <si>
@@ -472,12 +463,6 @@
     <t>Check if entering a valid email address sends the user's password to their email.</t>
   </si>
   <si>
-    <t>ForgotPassword_Tconn_1</t>
-  </si>
-  <si>
-    <t>JL</t>
-  </si>
-  <si>
     <t>The user will receive an email containing their password.</t>
   </si>
   <si>
@@ -496,9 +481,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>ForgotPassword_Tconn_3</t>
-  </si>
-  <si>
     <t>Go to page check for spelling or grammar mistakes.</t>
   </si>
   <si>
@@ -511,13 +493,40 @@
     <t>Email: InvalidEmail@qub.ac.uk</t>
   </si>
   <si>
-    <t>ForgotPassword_Tconn_2</t>
-  </si>
-  <si>
     <t>While on the forgot password page enter an invalid email address and click the send button.</t>
   </si>
   <si>
     <t>An appropriate validation message will appear.</t>
+  </si>
+  <si>
+    <t>To show that textual content in the email does not contain spelling or grammatical errors.</t>
+  </si>
+  <si>
+    <t>ForgotPassword_TConn_4</t>
+  </si>
+  <si>
+    <t>ForgotPassword_Tproc_4</t>
+  </si>
+  <si>
+    <t>ForgotPassword_TProc_3</t>
+  </si>
+  <si>
+    <t>ForgotPassword_TProc_2</t>
+  </si>
+  <si>
+    <t>ForgotPassword_TProc_1</t>
+  </si>
+  <si>
+    <t>Go to email check for spelling or grammar mistakes.</t>
+  </si>
+  <si>
+    <t>ForgotPassword_1</t>
+  </si>
+  <si>
+    <t>J Leathem</t>
+  </si>
+  <si>
+    <t>Email subject reads 'Bike IT - account details'. Should read 'Pizza IT - account details'.</t>
   </si>
 </sst>
 </file>
@@ -704,7 +713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -790,6 +799,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -930,7 +942,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1022,7 +1034,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1049,11 +1061,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1127205840"/>
-        <c:axId val="-1127194960"/>
+        <c:axId val="1138937808"/>
+        <c:axId val="1138934544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1127205840"/>
+        <c:axId val="1138937808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1063,7 +1075,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1127194960"/>
+        <c:crossAx val="1138934544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1071,7 +1083,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1127194960"/>
+        <c:axId val="1138934544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1082,7 +1094,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1127205840"/>
+        <c:crossAx val="1138937808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1490,8 +1502,8 @@
   </sheetPr>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,10 +1532,10 @@
         <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -1537,10 +1549,10 @@
         <v>59</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>27</v>
@@ -1552,10 +1564,10 @@
         <v>60</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>27</v>
@@ -1564,11 +1576,19 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="H5" s="6" t="s">
         <v>43</v>
       </c>
@@ -1656,7 +1676,7 @@
   <dimension ref="A1:Z161"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,16 +1752,16 @@
         <v>61</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>6</v>
@@ -1753,7 +1773,7 @@
         <v>24</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
@@ -1771,16 +1791,16 @@
         <v>62</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>27</v>
@@ -1792,7 +1812,7 @@
         <v>24</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="4"/>
@@ -1810,16 +1830,16 @@
         <v>63</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>27</v>
@@ -1831,7 +1851,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="4"/>
@@ -1851,17 +1871,39 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
+      <c r="E5" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="13">
+        <v>42101</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="33">
+        <v>42101</v>
+      </c>
+      <c r="N5" s="33">
+        <v>42101</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>96</v>
+      </c>
       <c r="P5" s="10"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -1954,7 +1996,7 @@
       </c>
       <c r="U9" s="32">
         <f>COUNTIF(H3:H90,"*Failed*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -2209,7 +2251,7 @@
       </c>
       <c r="U26" s="32">
         <f>COUNTIF(L2:L50,"*Minor*")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="5:21" x14ac:dyDescent="0.25">
@@ -4180,8 +4222,8 @@
   </sheetPr>
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4222,19 +4264,19 @@
     </row>
     <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F2" s="1"/>
       <c r="H2" s="28" t="s">
@@ -4248,19 +4290,19 @@
     </row>
     <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="1"/>
@@ -4273,16 +4315,16 @@
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -4294,11 +4336,19 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -4725,18 +4775,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4756,18 +4806,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Final Forgot Password Page
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 ForgotPasswordPage, Jonnie Leathem.xlsx
+++ b/Testing Spreadsheet v1.0 ForgotPasswordPage, Jonnie Leathem.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="16560" windowHeight="6345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -1393,13 +1393,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1500,7 +1500,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1515,11 +1515,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="161107792"/>
-        <c:axId val="161117040"/>
+        <c:axId val="1433862096"/>
+        <c:axId val="1433853936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="161107792"/>
+        <c:axId val="1433862096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1529,7 +1529,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161117040"/>
+        <c:crossAx val="1433853936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1537,7 +1537,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="161117040"/>
+        <c:axId val="1433853936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1548,7 +1548,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161107792"/>
+        <c:crossAx val="1433862096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1977,7 +1977,7 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -2304,8 +2304,8 @@
   </sheetPr>
   <dimension ref="A1:Z161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="K22" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2730,7 +2730,7 @@
       </c>
       <c r="U10" s="32">
         <f>COUNTIF(H2:H90,"*Passed*")</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="71.25" x14ac:dyDescent="0.25">
@@ -2816,7 +2816,7 @@
       </c>
       <c r="U12" s="32">
         <f>COUNTIF(H6:H90,"*Not*")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
@@ -2914,7 +2914,7 @@
         <v>42109</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>90</v>
@@ -2950,7 +2950,7 @@
         <v>42109</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>90</v>
@@ -3079,7 +3079,7 @@
         <v>233</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L19" s="4" t="s">
         <v>38</v>
@@ -3087,7 +3087,9 @@
       <c r="M19" s="33">
         <v>42109</v>
       </c>
-      <c r="N19" s="9"/>
+      <c r="N19" s="33">
+        <v>42110</v>
+      </c>
       <c r="O19" s="3" t="s">
         <v>208</v>
       </c>
@@ -3197,7 +3199,7 @@
         <v>245</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>38</v>
@@ -3205,7 +3207,9 @@
       <c r="M22" s="33">
         <v>42109</v>
       </c>
-      <c r="N22" s="9"/>
+      <c r="N22" s="33">
+        <v>42110</v>
+      </c>
       <c r="O22" s="3" t="s">
         <v>242</v>
       </c>
@@ -3294,7 +3298,7 @@
         <v>57</v>
       </c>
       <c r="U27" s="32">
-        <f>COUNTIF(L2:L9,"*Moderate*")</f>
+        <f>COUNTIF(L2:L50,"*Moderate*")</f>
         <v>0</v>
       </c>
     </row>
@@ -3315,7 +3319,7 @@
         <v>35</v>
       </c>
       <c r="U28" s="32">
-        <f>COUNTIF(L2:L9,"*Major*")</f>
+        <f>COUNTIF(L2:L50,"*Major*")</f>
         <v>0</v>
       </c>
     </row>
@@ -3336,7 +3340,7 @@
         <v>36</v>
       </c>
       <c r="U29" s="32">
-        <f>COUNTIF(L2:L9,"*Critical*")</f>
+        <f>COUNTIF(L2:L50,"*Critical*")</f>
         <v>0</v>
       </c>
     </row>
@@ -3357,8 +3361,8 @@
         <v>38</v>
       </c>
       <c r="U30" s="32">
-        <f>COUNTIF(L2:L9,"*Cometic*")</f>
-        <v>0</v>
+        <f>COUNTIF(L2:L50,"*Cosmetic*")</f>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -5207,7 +5211,7 @@
   <legacyDrawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Settings!$B$4:$B$6</xm:f>
@@ -5224,7 +5228,7 @@
           <x14:formula1>
             <xm:f>Settings!$D$4:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K13 K17</xm:sqref>
+          <xm:sqref>K2:K13 K17 K19 K22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -5248,12 +5252,6 @@
           <x14:formula1>
             <xm:f>[1]Settings!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>K19 K22</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>[1]Settings!#REF!</xm:f>
-          </x14:formula1>
           <xm:sqref>L19 L22 L17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
@@ -5269,7 +5267,7 @@
   </sheetPr>
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -5891,6 +5889,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -6004,15 +6011,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
   <ds:schemaRefs>
@@ -6023,6 +6021,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6036,12 +6042,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>